<commit_message>
fix: tempaltes laporan penjualan
</commit_message>
<xml_diff>
--- a/public/export_template/template_pembelian.xlsx
+++ b/public/export_template/template_pembelian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\storage\app\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF404BC1-1DE0-4FAE-91F4-05EB32A6DB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74FBEC4-F09F-4961-AB97-D53A74B76B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="3330" yWindow="1830" windowWidth="15375" windowHeight="8325" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,40 +44,46 @@
     <t>Jl. Tinumbu No.20 Telp (0411) 22099</t>
   </si>
   <si>
+    <t>Tanggal</t>
+  </si>
+  <si>
+    <t>Kode Barang</t>
+  </si>
+  <si>
+    <t>Merek</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>No Nota</t>
   </si>
   <si>
-    <t>Tanggal</t>
-  </si>
-  <si>
-    <t>Kode Barang</t>
-  </si>
-  <si>
     <t>Nama Barang</t>
   </si>
   <si>
-    <t>Merek</t>
-  </si>
-  <si>
     <t>Harga Satuan</t>
   </si>
   <si>
     <t xml:space="preserve">Jumlah </t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -99,41 +105,43 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{A3A5FC1B-5149-4B7A-B5E6-A11C8F05DA62}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,97 +473,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2042D607-C4CF-4B06-A3C3-62AF1890DECA}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: update date format to DD-MM-YYYY in Laporan Pembelian export and views
</commit_message>
<xml_diff>
--- a/public/export_template/template_pembelian.xlsx
+++ b/public/export_template/template_pembelian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74FBEC4-F09F-4961-AB97-D53A74B76B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FDA742-15F1-4B17-9664-23F58350A04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="1830" windowWidth="15375" windowHeight="8325" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,21 +123,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,92 +475,88 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>